<commit_message>
Commit with Test Scenario
Signed-off-by: ashaikh <ahmer.shaikh09@gmail.com>
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="UserDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="AdoptorDetails_Happy" sheetId="2" r:id="rId1"/>
+    <sheet name="AdoptorDetails_Negative" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -22,25 +23,58 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>ExcelLast</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Field Name</t>
   </si>
   <si>
     <t>Field Value</t>
   </si>
   <si>
-    <t>ExcelFirst</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>def@ghi.com</t>
+  </si>
+  <si>
+    <t>Address Line</t>
+  </si>
+  <si>
+    <t>Optional Address</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>The quick fox jumps over lazy dog…</t>
+  </si>
+  <si>
+    <t>wrongemail</t>
   </si>
 </sst>
 </file>
@@ -50,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +95,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,15 +131,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C5"/>
+  <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,47 +467,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43252</v>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="def@ghi.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>